<commit_message>
Actualizando cronograma según avance
</commit_message>
<xml_diff>
--- a/Desarrollo/Gestion/SGDS - CP.XLS.xlsx
+++ b/Desarrollo/Gestion/SGDS - CP.XLS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup\Escritorio\QuantumAnts Software\QuantumAnts-Software\Desarrollo\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A2F984-B1D6-452E-9603-5D27A0CB98EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C897912-8345-49CD-B53F-A5628996DACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -706,7 +706,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="49">
+  <fonts count="50">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -999,6 +999,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1446,7 +1453,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1650,19 +1657,6 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1684,6 +1678,20 @@
     <xf numFmtId="0" fontId="44" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1905,7 +1913,7 @@
   </sheetPr>
   <dimension ref="A1:K998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1916,29 +1924,30 @@
     <col min="3" max="3" width="52.140625" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
     <col min="5" max="5" width="81.5703125" customWidth="1"/>
-    <col min="6" max="7" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="10.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="106"/>
+      <c r="C2" s="114"/>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="3"/>
@@ -1996,7 +2005,7 @@
         <v>45022</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="117"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="4"/>
@@ -2033,7 +2042,7 @@
       <c r="C9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="110" t="s">
+      <c r="D9" s="103" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="14" t="s">
@@ -2059,7 +2068,7 @@
       <c r="C10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="111" t="s">
+      <c r="D10" s="104" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="18" t="s">
@@ -2085,7 +2094,7 @@
       <c r="C11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="111" t="s">
+      <c r="D11" s="104" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="18" t="s">
@@ -2113,7 +2122,7 @@
       <c r="C12" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="111" t="s">
+      <c r="D12" s="104" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="18" t="s">
@@ -2128,7 +2137,7 @@
       <c r="H12" s="20">
         <v>1</v>
       </c>
-      <c r="I12" s="107" t="s">
+      <c r="I12" s="110" t="s">
         <v>25</v>
       </c>
       <c r="J12" s="2"/>
@@ -2142,7 +2151,7 @@
       <c r="C13" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="111" t="s">
+      <c r="D13" s="104" t="s">
         <v>28</v>
       </c>
       <c r="E13" s="29" t="s">
@@ -2157,7 +2166,7 @@
       <c r="H13" s="20">
         <v>1</v>
       </c>
-      <c r="I13" s="104"/>
+      <c r="I13" s="111"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
@@ -2168,7 +2177,7 @@
       <c r="C14" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="111" t="s">
+      <c r="D14" s="104" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="29" t="s">
@@ -2183,7 +2192,7 @@
       <c r="H14" s="20">
         <v>1</v>
       </c>
-      <c r="I14" s="104"/>
+      <c r="I14" s="111"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
@@ -2194,7 +2203,7 @@
       <c r="C15" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="111" t="s">
+      <c r="D15" s="104" t="s">
         <v>35</v>
       </c>
       <c r="E15" s="32" t="s">
@@ -2206,10 +2215,10 @@
       <c r="G15" s="31">
         <v>45036</v>
       </c>
-      <c r="H15" s="33">
-        <v>0</v>
-      </c>
-      <c r="I15" s="104"/>
+      <c r="H15" s="20">
+        <v>1</v>
+      </c>
+      <c r="I15" s="111"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
@@ -2221,7 +2230,7 @@
       <c r="C16" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="111" t="s">
+      <c r="D16" s="104" t="s">
         <v>39</v>
       </c>
       <c r="E16" s="29" t="s">
@@ -2233,10 +2242,10 @@
       <c r="G16" s="31">
         <v>45036</v>
       </c>
-      <c r="H16" s="33">
-        <v>0</v>
-      </c>
-      <c r="I16" s="104"/>
+      <c r="H16" s="20">
+        <v>1</v>
+      </c>
+      <c r="I16" s="111"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
@@ -2248,7 +2257,7 @@
       <c r="C17" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="111" t="s">
+      <c r="D17" s="104" t="s">
         <v>43</v>
       </c>
       <c r="E17" s="29" t="s">
@@ -2260,10 +2269,10 @@
       <c r="G17" s="31">
         <v>45036</v>
       </c>
-      <c r="H17" s="33">
-        <v>0</v>
-      </c>
-      <c r="I17" s="104"/>
+      <c r="H17" s="20">
+        <v>1</v>
+      </c>
+      <c r="I17" s="111"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
@@ -2275,7 +2284,7 @@
       <c r="C18" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="111" t="s">
+      <c r="D18" s="104" t="s">
         <v>47</v>
       </c>
       <c r="E18" s="29" t="s">
@@ -2287,10 +2296,10 @@
       <c r="G18" s="31">
         <v>45036</v>
       </c>
-      <c r="H18" s="33">
-        <v>0</v>
-      </c>
-      <c r="I18" s="104"/>
+      <c r="H18" s="20">
+        <v>1</v>
+      </c>
+      <c r="I18" s="111"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
@@ -2302,7 +2311,7 @@
       <c r="C19" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="111" t="s">
+      <c r="D19" s="104" t="s">
         <v>50</v>
       </c>
       <c r="E19" s="32" t="s">
@@ -2314,10 +2323,10 @@
       <c r="G19" s="31">
         <v>45036</v>
       </c>
-      <c r="H19" s="33">
-        <v>0</v>
-      </c>
-      <c r="I19" s="104"/>
+      <c r="H19" s="20">
+        <v>1</v>
+      </c>
+      <c r="I19" s="111"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
@@ -2329,7 +2338,7 @@
       <c r="C20" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="111" t="s">
+      <c r="D20" s="104" t="s">
         <v>53</v>
       </c>
       <c r="E20" s="32" t="s">
@@ -2341,10 +2350,10 @@
       <c r="G20" s="31">
         <v>45036</v>
       </c>
-      <c r="H20" s="33">
-        <v>0</v>
-      </c>
-      <c r="I20" s="104"/>
+      <c r="H20" s="20">
+        <v>1</v>
+      </c>
+      <c r="I20" s="111"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
@@ -2356,7 +2365,7 @@
       <c r="C21" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="111" t="s">
+      <c r="D21" s="104" t="s">
         <v>56</v>
       </c>
       <c r="E21" s="29" t="s">
@@ -2368,10 +2377,10 @@
       <c r="G21" s="31">
         <v>45036</v>
       </c>
-      <c r="H21" s="33">
-        <v>0</v>
-      </c>
-      <c r="I21" s="104"/>
+      <c r="H21" s="20">
+        <v>1</v>
+      </c>
+      <c r="I21" s="111"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
@@ -2383,7 +2392,7 @@
       <c r="C22" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="111" t="s">
+      <c r="D22" s="104" t="s">
         <v>60</v>
       </c>
       <c r="E22" s="32" t="s">
@@ -2395,10 +2404,10 @@
       <c r="G22" s="31">
         <v>45036</v>
       </c>
-      <c r="H22" s="33">
-        <v>0</v>
-      </c>
-      <c r="I22" s="104"/>
+      <c r="H22" s="20">
+        <v>1</v>
+      </c>
+      <c r="I22" s="111"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
@@ -2410,7 +2419,7 @@
       <c r="C23" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="111" t="s">
+      <c r="D23" s="104" t="s">
         <v>63</v>
       </c>
       <c r="E23" s="32" t="s">
@@ -2422,10 +2431,10 @@
       <c r="G23" s="31">
         <v>45036</v>
       </c>
-      <c r="H23" s="33">
-        <v>0</v>
-      </c>
-      <c r="I23" s="104"/>
+      <c r="H23" s="20">
+        <v>1</v>
+      </c>
+      <c r="I23" s="111"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
@@ -2437,7 +2446,7 @@
       <c r="C24" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="111" t="s">
+      <c r="D24" s="104" t="s">
         <v>165</v>
       </c>
       <c r="E24" s="29" t="s">
@@ -2449,8 +2458,8 @@
       <c r="G24" s="31">
         <v>45040</v>
       </c>
-      <c r="H24" s="33">
-        <v>0</v>
+      <c r="H24" s="20">
+        <v>1</v>
       </c>
       <c r="I24" s="21"/>
       <c r="J24" s="2"/>
@@ -2464,7 +2473,7 @@
       <c r="C25" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="111" t="s">
+      <c r="D25" s="104" t="s">
         <v>166</v>
       </c>
       <c r="E25" s="29" t="s">
@@ -2476,8 +2485,8 @@
       <c r="G25" s="31">
         <v>45044</v>
       </c>
-      <c r="H25" s="33">
-        <v>0</v>
+      <c r="H25" s="20">
+        <v>1</v>
       </c>
       <c r="I25" s="21"/>
       <c r="J25" s="2"/>
@@ -2491,7 +2500,7 @@
       <c r="C26" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="111" t="s">
+      <c r="D26" s="104" t="s">
         <v>167</v>
       </c>
       <c r="E26" s="29" t="s">
@@ -2503,10 +2512,10 @@
       <c r="G26" s="31">
         <v>45048</v>
       </c>
-      <c r="H26" s="33">
-        <v>0</v>
-      </c>
-      <c r="I26" s="107" t="s">
+      <c r="H26" s="20">
+        <v>1</v>
+      </c>
+      <c r="I26" s="110" t="s">
         <v>73</v>
       </c>
       <c r="J26" s="2"/>
@@ -2520,7 +2529,7 @@
       <c r="C27" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="111" t="s">
+      <c r="D27" s="104" t="s">
         <v>76</v>
       </c>
       <c r="E27" s="29" t="s">
@@ -2535,7 +2544,7 @@
       <c r="H27" s="33">
         <v>0</v>
       </c>
-      <c r="I27" s="104"/>
+      <c r="I27" s="111"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
@@ -2547,7 +2556,7 @@
       <c r="C28" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="111" t="s">
+      <c r="D28" s="104" t="s">
         <v>168</v>
       </c>
       <c r="E28" s="29" t="s">
@@ -2562,7 +2571,7 @@
       <c r="H28" s="33">
         <v>0</v>
       </c>
-      <c r="I28" s="107" t="s">
+      <c r="I28" s="110" t="s">
         <v>80</v>
       </c>
       <c r="J28" s="2"/>
@@ -2576,7 +2585,7 @@
       <c r="C29" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="D29" s="111" t="s">
+      <c r="D29" s="104" t="s">
         <v>83</v>
       </c>
       <c r="E29" s="29" t="s">
@@ -2591,7 +2600,7 @@
       <c r="H29" s="33">
         <v>0</v>
       </c>
-      <c r="I29" s="104"/>
+      <c r="I29" s="111"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
@@ -2603,7 +2612,7 @@
         <v>85</v>
       </c>
       <c r="C30" s="40"/>
-      <c r="D30" s="112"/>
+      <c r="D30" s="105"/>
       <c r="E30" s="41"/>
       <c r="F30" s="42">
         <v>45052</v>
@@ -2613,9 +2622,9 @@
       </c>
       <c r="H30" s="43">
         <f>SUM(H10:H29)/21</f>
-        <v>0.23809523809523808</v>
-      </c>
-      <c r="I30" s="104"/>
+        <v>0.80952380952380953</v>
+      </c>
+      <c r="I30" s="111"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A31" s="9"/>
@@ -2625,7 +2634,7 @@
       <c r="C31" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="D31" s="113" t="s">
+      <c r="D31" s="106" t="s">
         <v>169</v>
       </c>
       <c r="E31" s="32" t="s">
@@ -2654,7 +2663,7 @@
       <c r="C32" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="113" t="s">
+      <c r="D32" s="106" t="s">
         <v>170</v>
       </c>
       <c r="E32" s="32" t="s">
@@ -2681,7 +2690,7 @@
       <c r="C33" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="113" t="s">
+      <c r="D33" s="106" t="s">
         <v>171</v>
       </c>
       <c r="E33" s="29" t="s">
@@ -2708,7 +2717,7 @@
       <c r="C34" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="114" t="s">
+      <c r="D34" s="107" t="s">
         <v>172</v>
       </c>
       <c r="E34" s="32" t="s">
@@ -2735,7 +2744,7 @@
       <c r="C35" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="114" t="s">
+      <c r="D35" s="107" t="s">
         <v>173</v>
       </c>
       <c r="E35" s="50" t="s">
@@ -2762,7 +2771,7 @@
       <c r="C36" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="111" t="s">
+      <c r="D36" s="104" t="s">
         <v>167</v>
       </c>
       <c r="E36" s="50" t="s">
@@ -2789,7 +2798,7 @@
       <c r="C37" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="115" t="s">
+      <c r="D37" s="108" t="s">
         <v>174</v>
       </c>
       <c r="E37" s="50" t="s">
@@ -2804,7 +2813,7 @@
       <c r="H37" s="54">
         <v>0</v>
       </c>
-      <c r="I37" s="107" t="s">
+      <c r="I37" s="110" t="s">
         <v>96</v>
       </c>
       <c r="J37" s="47"/>
@@ -2818,7 +2827,7 @@
       <c r="C38" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="D38" s="111" t="s">
+      <c r="D38" s="104" t="s">
         <v>98</v>
       </c>
       <c r="E38" s="29" t="s">
@@ -2833,7 +2842,7 @@
       <c r="H38" s="54">
         <v>0</v>
       </c>
-      <c r="I38" s="104"/>
+      <c r="I38" s="111"/>
       <c r="J38" s="47"/>
       <c r="K38" s="2"/>
     </row>
@@ -2845,7 +2854,7 @@
         <v>100</v>
       </c>
       <c r="C39" s="56"/>
-      <c r="D39" s="112"/>
+      <c r="D39" s="105"/>
       <c r="E39" s="57"/>
       <c r="F39" s="58">
         <v>45061</v>
@@ -2857,7 +2866,7 @@
         <f>SUM(H31:H38)/9</f>
         <v>0</v>
       </c>
-      <c r="I39" s="104"/>
+      <c r="I39" s="111"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A40" s="9"/>
@@ -2867,7 +2876,7 @@
       <c r="C40" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="D40" s="115" t="s">
+      <c r="D40" s="108" t="s">
         <v>175</v>
       </c>
       <c r="E40" s="29" t="s">
@@ -2894,7 +2903,7 @@
       <c r="C41" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="D41" s="115" t="s">
+      <c r="D41" s="108" t="s">
         <v>176</v>
       </c>
       <c r="E41" s="32" t="s">
@@ -2921,7 +2930,7 @@
       <c r="C42" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="D42" s="115" t="s">
+      <c r="D42" s="108" t="s">
         <v>177</v>
       </c>
       <c r="E42" s="32" t="s">
@@ -2948,7 +2957,7 @@
       <c r="C43" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="D43" s="115" t="s">
+      <c r="D43" s="108" t="s">
         <v>178</v>
       </c>
       <c r="E43" s="29" t="s">
@@ -2975,7 +2984,7 @@
       <c r="C44" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="D44" s="115" t="s">
+      <c r="D44" s="108" t="s">
         <v>179</v>
       </c>
       <c r="E44" s="32" t="s">
@@ -3002,7 +3011,7 @@
       <c r="C45" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="D45" s="115" t="s">
+      <c r="D45" s="108" t="s">
         <v>180</v>
       </c>
       <c r="E45" s="32" t="s">
@@ -3029,7 +3038,7 @@
       <c r="C46" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="D46" s="111" t="s">
+      <c r="D46" s="104" t="s">
         <v>114</v>
       </c>
       <c r="E46" s="32" t="s">
@@ -3056,7 +3065,7 @@
       <c r="C47" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="D47" s="115" t="s">
+      <c r="D47" s="108" t="s">
         <v>181</v>
       </c>
       <c r="E47" s="50" t="s">
@@ -3083,7 +3092,7 @@
       <c r="C48" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="D48" s="111" t="s">
+      <c r="D48" s="104" t="s">
         <v>116</v>
       </c>
       <c r="E48" s="50" t="s">
@@ -3110,7 +3119,7 @@
       <c r="C49" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="D49" s="111" t="s">
+      <c r="D49" s="104" t="s">
         <v>119</v>
       </c>
       <c r="E49" s="50" t="s">
@@ -3125,7 +3134,7 @@
       <c r="H49" s="54">
         <v>0</v>
       </c>
-      <c r="I49" s="107" t="s">
+      <c r="I49" s="110" t="s">
         <v>120</v>
       </c>
       <c r="J49" s="47"/>
@@ -3139,7 +3148,7 @@
       <c r="C50" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="D50" s="115" t="s">
+      <c r="D50" s="108" t="s">
         <v>182</v>
       </c>
       <c r="E50" s="50" t="s">
@@ -3154,7 +3163,7 @@
       <c r="H50" s="54">
         <v>0</v>
       </c>
-      <c r="I50" s="104"/>
+      <c r="I50" s="111"/>
       <c r="J50" s="47"/>
       <c r="K50" s="2"/>
     </row>
@@ -3166,7 +3175,7 @@
       <c r="C51" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="D51" s="111" t="s">
+      <c r="D51" s="104" t="s">
         <v>122</v>
       </c>
       <c r="E51" s="50" t="s">
@@ -3181,7 +3190,7 @@
       <c r="H51" s="54">
         <v>0</v>
       </c>
-      <c r="I51" s="107" t="s">
+      <c r="I51" s="110" t="s">
         <v>123</v>
       </c>
       <c r="J51" s="47"/>
@@ -3195,7 +3204,7 @@
       <c r="C52" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="D52" s="111" t="s">
+      <c r="D52" s="104" t="s">
         <v>126</v>
       </c>
       <c r="E52" s="50" t="s">
@@ -3210,7 +3219,7 @@
       <c r="H52" s="54">
         <v>0</v>
       </c>
-      <c r="I52" s="104"/>
+      <c r="I52" s="111"/>
       <c r="J52" s="47"/>
       <c r="K52" s="2"/>
     </row>
@@ -3222,7 +3231,7 @@
         <v>128</v>
       </c>
       <c r="C53" s="67"/>
-      <c r="D53" s="116"/>
+      <c r="D53" s="109"/>
       <c r="E53" s="68"/>
       <c r="F53" s="69">
         <f>F40</f>
@@ -3236,7 +3245,7 @@
         <f>SUM(H40:H52)/13</f>
         <v>0</v>
       </c>
-      <c r="I53" s="104"/>
+      <c r="I53" s="111"/>
     </row>
     <row r="54" spans="1:11" ht="15.75" customHeight="1">
       <c r="B54" s="22"/>
@@ -5040,10 +5049,10 @@
       <c r="C2" s="9"/>
     </row>
     <row r="3" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="115" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="109"/>
+      <c r="C3" s="116"/>
     </row>
     <row r="4" spans="2:3" ht="15.75" customHeight="1">
       <c r="B4" s="74" t="s">

</xml_diff>